<commit_message>
Added: Phaser3 Sprite test
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B074D23-E979-4333-B91A-601CF07AD718}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3847F816-5CFF-409D-9AFF-5ED13FC050CF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Amount</t>
   </si>
@@ -29,6 +35,21 @@
   </si>
   <si>
     <t>Phaser 3: Blitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Som</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
+  </si>
+  <si>
+    <t>Voorlopig totaal</t>
+  </si>
+  <si>
+    <t>Aantal</t>
   </si>
 </sst>
 </file>
@@ -60,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -68,17 +89,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -359,92 +509,597 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="9">
         <v>500</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="C4" s="10">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5">
         <v>1000</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="C5" s="6">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5">
         <v>1500</v>
       </c>
+      <c r="C6" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7" s="5">
         <v>2000</v>
       </c>
+      <c r="C7" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
       <c r="B8" s="5">
         <v>2500</v>
       </c>
+      <c r="C8" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9" s="5">
         <v>3000</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="C9" s="6">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="5">
         <v>3500</v>
       </c>
+      <c r="C10" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11" s="5">
         <v>4000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>4500</v>
       </c>
+      <c r="C12" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>5000</v>
+      </c>
+      <c r="C13" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>5500</v>
+      </c>
+      <c r="C14" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>6000</v>
+      </c>
+      <c r="C15" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>6500</v>
+      </c>
+      <c r="C16" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>7000</v>
+      </c>
+      <c r="C17" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>7500</v>
+      </c>
+      <c r="C18" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>8000</v>
+      </c>
+      <c r="C19" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>8500</v>
+      </c>
+      <c r="C20" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>9000</v>
+      </c>
+      <c r="C21" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>9500</v>
+      </c>
+      <c r="C22" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C23" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>10500</v>
+      </c>
+      <c r="C24" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>11000</v>
+      </c>
+      <c r="C25" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>11500</v>
+      </c>
+      <c r="C26" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>12000</v>
+      </c>
+      <c r="C27" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>12500</v>
+      </c>
+      <c r="C28" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>13000</v>
+      </c>
+      <c r="C29" s="6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>13500</v>
+      </c>
+      <c r="C30" s="6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>14000</v>
+      </c>
+      <c r="C31" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>14500</v>
+      </c>
+      <c r="C32" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
+        <v>15000</v>
+      </c>
+      <c r="C33" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
+        <v>15500</v>
+      </c>
+      <c r="C34" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>16000</v>
+      </c>
+      <c r="C35" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
+        <v>16500</v>
+      </c>
+      <c r="C36" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
+        <v>17000</v>
+      </c>
+      <c r="C37" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
+        <v>17500</v>
+      </c>
+      <c r="C38" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="5">
+        <v>18000</v>
+      </c>
+      <c r="C39" s="6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="5">
+        <v>18500</v>
+      </c>
+      <c r="C40" s="6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
+        <v>19000</v>
+      </c>
+      <c r="C41" s="6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
+        <v>19500</v>
+      </c>
+      <c r="C42" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="5">
+        <v>20000</v>
+      </c>
+      <c r="C43" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="5">
+        <v>20500</v>
+      </c>
+      <c r="C44" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="5">
+        <v>21000</v>
+      </c>
+      <c r="C45" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
+        <v>21500</v>
+      </c>
+      <c r="C46" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
+        <v>22000</v>
+      </c>
+      <c r="C47" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="5">
+        <v>22500</v>
+      </c>
+      <c r="C48" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
+        <v>23000</v>
+      </c>
+      <c r="C49" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
+        <v>23500</v>
+      </c>
+      <c r="C50" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
+        <v>24000</v>
+      </c>
+      <c r="C51" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>24500</v>
+      </c>
+      <c r="C52" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <v>25000</v>
+      </c>
+      <c r="C53" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>